<commit_message>
Updated analysis for darkness condition after adding more N
</commit_message>
<xml_diff>
--- a/Data/behaviour/generalization/Darkness.xlsx
+++ b/Data/behaviour/generalization/Darkness.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/lab-kohlj/home/users/borakn/Data/Behaviour/Generalisation Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/lab-kohlj/home/shared/projects/HierarchySensoryModality/Code/Data/behaviour/generalization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9E600F-9FC1-A84A-B60F-114684BF631E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BC8A40-1FB9-D74D-AC52-F72B9B5570D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="5380" windowWidth="28800" windowHeight="16280" xr2:uid="{29A28DD6-B1C1-FC42-8266-32BC55A4AA70}"/>
+    <workbookView xWindow="640" yWindow="1580" windowWidth="10000" windowHeight="16280" xr2:uid="{29A28DD6-B1C1-FC42-8266-32BC55A4AA70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -141,7 +141,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -247,7 +247,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -389,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FAAF97-9FB6-8D4C-9CF7-C3A703BDE243}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,6 +693,358 @@
         <v>1</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>